<commit_message>
Hunting for errors in data extraction
</commit_message>
<xml_diff>
--- a/preprocessing/possible_ranges_for_variables.xlsx
+++ b/preprocessing/possible_ranges_for_variables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jk1/stroke_research/OPSUM/preprocessing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97504C19-2DFF-8142-A47B-DF9C1E00F833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76997F2B-A924-6F49-A66A-CC9172158D17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="500" windowWidth="19200" windowHeight="21100" tabRatio="204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" tabRatio="204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PDFTables.com" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="61">
   <si>
     <t>Min</t>
   </si>
@@ -139,9 +139,6 @@
     <t>units</t>
   </si>
   <si>
-    <t xml:space="preserve">creatinine </t>
-  </si>
-  <si>
     <t>(umol/L)</t>
   </si>
   <si>
@@ -194,12 +191,27 @@
   </si>
   <si>
     <t>FIO2</t>
+  </si>
+  <si>
+    <t>Serum glucose</t>
+  </si>
+  <si>
+    <t>glucose</t>
+  </si>
+  <si>
+    <t>mmol/l</t>
+  </si>
+  <si>
+    <t>creatinine</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -237,7 +249,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -250,6 +262,8 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -589,10 +603,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -605,7 +619,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>21</v>
@@ -631,7 +645,7 @@
         <v>22</v>
       </c>
       <c r="D2" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E2" s="1">
         <v>120</v>
@@ -673,7 +687,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D5" s="1">
         <v>21</v>
@@ -684,10 +698,10 @@
     </row>
     <row r="6" spans="1:6" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>54</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>55</v>
       </c>
       <c r="D6" s="10">
         <v>0</v>
@@ -698,10 +712,10 @@
     </row>
     <row r="7" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D7" s="1">
         <v>3</v>
@@ -715,7 +729,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D8" s="1">
         <v>25</v>
@@ -758,7 +772,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D11" s="1">
         <v>10</v>
@@ -812,13 +826,13 @@
     </row>
     <row r="15" spans="1:6" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="C15" s="8" t="s">
         <v>50</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>51</v>
       </c>
       <c r="D15" s="9">
         <v>40</v>
@@ -832,7 +846,7 @@
         <v>10</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D16" s="1">
         <v>3</v>
@@ -841,176 +855,194 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" s="1">
-        <v>2</v>
-      </c>
-      <c r="E17" s="1">
-        <v>55</v>
+    <row r="17" spans="1:5" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="E17" s="11">
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>40</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="C18" s="8"/>
       <c r="D18" s="1">
-        <v>0</v>
-      </c>
-      <c r="E18" s="2">
-        <v>14000</v>
+        <v>2</v>
+      </c>
+      <c r="E18" s="1">
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D19">
-        <v>0.9</v>
-      </c>
-      <c r="E19" s="1">
-        <v>15</v>
+        <v>60</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0</v>
+      </c>
+      <c r="E19" s="2">
+        <v>14000</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D20" s="1">
-        <v>95</v>
+        <v>29</v>
+      </c>
+      <c r="D20">
+        <v>0.9</v>
       </c>
       <c r="E20" s="1">
-        <v>175</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="1">
+        <v>95</v>
+      </c>
+      <c r="E21" s="1">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B22" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D22" s="1">
         <v>1</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E22" s="1">
         <v>80</v>
       </c>
     </row>
-    <row r="22" spans="1:5" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="8" t="s">
+    <row r="23" spans="1:5" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D22" s="7">
+      <c r="D23" s="7">
         <v>0</v>
       </c>
-      <c r="E22" s="7">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" t="s">
-        <v>16</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D23" s="1">
-        <v>0</v>
-      </c>
-      <c r="E23" s="1">
+      <c r="E23" s="7">
         <v>300</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>42</v>
       </c>
       <c r="D24" s="1">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="E24" s="1">
-        <v>43</v>
+        <v>300</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" s="1">
+        <v>24</v>
+      </c>
+      <c r="E25" s="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" t="s">
         <v>18</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D26" s="1">
         <v>0</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E26" s="2">
         <v>20000</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="8" t="s">
+    <row r="27" spans="1:5" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B26" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D26" s="9">
+      <c r="D27" s="9">
         <v>20</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E27" s="2">
         <v>250</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" t="s">
+    <row r="28" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" t="s">
         <v>19</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B28" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D28" s="1">
         <v>0</v>
       </c>
-      <c r="E27" s="2">
+      <c r="E28" s="2">
         <v>1000</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="11"/>
-      <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-    </row>
     <row r="29" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="8"/>
+      <c r="A29" s="12"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+    </row>
+    <row r="30" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A28:E28"/>
+    <mergeCell ref="A29:E29"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Updated lab preprocessing to 06 2022 extraction
</commit_message>
<xml_diff>
--- a/preprocessing/possible_ranges_for_variables.xlsx
+++ b/preprocessing/possible_ranges_for_variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jk1/stroke_research/OPSUM/preprocessing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76997F2B-A924-6F49-A66A-CC9172158D17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34887EDA-52DA-B944-9FE2-E5FD16288C6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" tabRatio="204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="500" windowWidth="19200" windowHeight="21100" tabRatio="204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PDFTables.com" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="62">
   <si>
     <t>Min</t>
   </si>
@@ -94,9 +94,6 @@
     <t>G-Sgv-pH(T), ABL</t>
   </si>
   <si>
-    <t>actually venous pH for now</t>
-  </si>
-  <si>
     <t>bilirubine totale</t>
   </si>
   <si>
@@ -203,6 +200,12 @@
   </si>
   <si>
     <t>creatinine</t>
+  </si>
+  <si>
+    <t>thrombocytes</t>
+  </si>
+  <si>
+    <t>G/l</t>
   </si>
 </sst>
 </file>
@@ -249,7 +252,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -264,6 +267,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -606,7 +610,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -619,13 +623,13 @@
   <sheetData>
     <row r="1" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>0</v>
@@ -634,7 +638,7 @@
         <v>1</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -664,16 +668,13 @@
       <c r="E3">
         <v>7.8</v>
       </c>
-      <c r="F3" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="4" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D4" s="1">
         <v>1</v>
@@ -687,7 +688,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D5" s="1">
         <v>21</v>
@@ -698,10 +699,10 @@
     </row>
     <row r="6" spans="1:6" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>53</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>54</v>
       </c>
       <c r="D6" s="10">
         <v>0</v>
@@ -712,10 +713,10 @@
     </row>
     <row r="7" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D7" s="1">
         <v>3</v>
@@ -729,7 +730,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D8" s="1">
         <v>25</v>
@@ -743,7 +744,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D9" s="1">
         <v>5</v>
@@ -754,10 +755,10 @@
     </row>
     <row r="10" spans="1:6" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>36</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="4">
@@ -772,7 +773,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D11" s="1">
         <v>10</v>
@@ -786,7 +787,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D12" s="1">
         <v>1</v>
@@ -800,7 +801,7 @@
         <v>9</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D13" s="1">
         <v>4</v>
@@ -811,10 +812,10 @@
     </row>
     <row r="14" spans="1:6" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="4">
@@ -826,13 +827,13 @@
     </row>
     <row r="15" spans="1:6" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="C15" s="8" t="s">
         <v>49</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>50</v>
       </c>
       <c r="D15" s="9">
         <v>40</v>
@@ -846,7 +847,7 @@
         <v>10</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D16" s="1">
         <v>3</v>
@@ -857,13 +858,13 @@
     </row>
     <row r="17" spans="1:5" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="C17" s="8" t="s">
         <v>58</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>59</v>
       </c>
       <c r="D17" s="13">
         <v>0.5</v>
@@ -889,10 +890,10 @@
         <v>12</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D19" s="1">
         <v>0</v>
@@ -906,7 +907,7 @@
         <v>13</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D20">
         <v>0.9</v>
@@ -920,7 +921,7 @@
         <v>14</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D21" s="1">
         <v>95</v>
@@ -934,7 +935,7 @@
         <v>15</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D22" s="1">
         <v>1</v>
@@ -945,10 +946,10 @@
     </row>
     <row r="23" spans="1:5" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="8" t="s">
         <v>43</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>44</v>
       </c>
       <c r="D23" s="7">
         <v>0</v>
@@ -962,7 +963,7 @@
         <v>16</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D24" s="1">
         <v>0</v>
@@ -976,7 +977,7 @@
         <v>17</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D25" s="1">
         <v>24</v>
@@ -998,13 +999,13 @@
     </row>
     <row r="27" spans="1:5" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="8" t="s">
         <v>51</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>52</v>
       </c>
       <c r="D27" s="9">
         <v>20</v>
@@ -1018,7 +1019,7 @@
         <v>19</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D28" s="1">
         <v>0</v>
@@ -1028,19 +1029,26 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="12"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
+      <c r="A29" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="D29" s="12">
+        <v>0</v>
+      </c>
+      <c r="E29" s="2">
+        <v>1000</v>
+      </c>
     </row>
     <row r="30" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A29:E29"/>
-  </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0"/>
   <headerFooter>

</xml_diff>

<commit_message>
Updated preprocessing of patientValues (vitals) for extraction of 08 2022
</commit_message>
<xml_diff>
--- a/preprocessing/possible_ranges_for_variables.xlsx
+++ b/preprocessing/possible_ranges_for_variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jk1/stroke_research/OPSUM/preprocessing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34887EDA-52DA-B944-9FE2-E5FD16288C6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3F4AE64-B227-374E-99BB-4E93CA109F6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="500" windowWidth="19200" windowHeight="21100" tabRatio="204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="8780" windowWidth="21100" windowHeight="12820" tabRatio="204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PDFTables.com" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="64">
   <si>
     <t>Min</t>
   </si>
@@ -206,6 +206,12 @@
   </si>
   <si>
     <t>G/l</t>
+  </si>
+  <si>
+    <t>bpm</t>
+  </si>
+  <si>
+    <t>/min</t>
   </si>
 </sst>
 </file>
@@ -609,8 +615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="B17" zoomScale="169" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -690,6 +696,9 @@
       <c r="B5" s="3" t="s">
         <v>55</v>
       </c>
+      <c r="C5" s="5" t="s">
+        <v>49</v>
+      </c>
       <c r="D5" s="1">
         <v>21</v>
       </c>
@@ -732,6 +741,9 @@
       <c r="B8" s="3" t="s">
         <v>45</v>
       </c>
+      <c r="C8" s="5" t="s">
+        <v>62</v>
+      </c>
       <c r="D8" s="1">
         <v>25</v>
       </c>
@@ -848,6 +860,9 @@
       </c>
       <c r="B16" s="3" t="s">
         <v>46</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>63</v>
       </c>
       <c r="D16" s="1">
         <v>3</v>

</xml_diff>